<commit_message>
show values in game over, new excel
</commit_message>
<xml_diff>
--- a/sg_values.xlsx
+++ b/sg_values.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiri\Documents\טכניון\תזה\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiri\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14030" windowHeight="7530" xr2:uid="{37C38814-6A3B-4419-BA12-908521172DDA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="7530" xr2:uid="{37C38814-6A3B-4419-BA12-908521172DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="game values" sheetId="1" r:id="rId1"/>
@@ -1465,15 +1465,6 @@
           <cell r="O50">
             <v>-298.6832887881805</v>
           </cell>
-          <cell r="R50">
-            <v>7.674908222697073E-2</v>
-          </cell>
-          <cell r="S50">
-            <v>0.44652224277684377</v>
-          </cell>
-          <cell r="T50">
-            <v>13.162319618786457</v>
-          </cell>
         </row>
         <row r="51">
           <cell r="C51">
@@ -1503,15 +1494,6 @@
           <cell r="O51">
             <v>-1.8790380617984361</v>
           </cell>
-          <cell r="R51">
-            <v>0.84484862289422646</v>
-          </cell>
-          <cell r="S51">
-            <v>0.49964717978523288</v>
-          </cell>
-          <cell r="T51">
-            <v>53.928453808363962</v>
-          </cell>
         </row>
         <row r="52">
           <cell r="C52">
@@ -1541,15 +1523,6 @@
           <cell r="O52">
             <v>-292.2020275895614</v>
           </cell>
-          <cell r="R52">
-            <v>0.19891097288966214</v>
-          </cell>
-          <cell r="S52">
-            <v>0.43134861960005549</v>
-          </cell>
-          <cell r="T52">
-            <v>19.998745552168764</v>
-          </cell>
         </row>
         <row r="53">
           <cell r="C53">
@@ -1579,15 +1552,6 @@
           <cell r="O53">
             <v>10.465555987243157</v>
           </cell>
-          <cell r="R53">
-            <v>0.16951811053240545</v>
-          </cell>
-          <cell r="S53">
-            <v>0.49691995723536803</v>
-          </cell>
-          <cell r="T53">
-            <v>46.916546595343952</v>
-          </cell>
         </row>
         <row r="54">
           <cell r="C54">
@@ -1617,15 +1581,6 @@
           <cell r="O54">
             <v>-36.626966224120913</v>
           </cell>
-          <cell r="R54">
-            <v>0.89268779044524482</v>
-          </cell>
-          <cell r="S54">
-            <v>0.41407106591789594</v>
-          </cell>
-          <cell r="T54">
-            <v>17.414228768631862</v>
-          </cell>
         </row>
         <row r="55">
           <cell r="C55">
@@ -1655,15 +1610,6 @@
           <cell r="O55">
             <v>3.3345245803765438</v>
           </cell>
-          <cell r="R55">
-            <v>0.13441082487941508</v>
-          </cell>
-          <cell r="S55">
-            <v>0.45174069708711406</v>
-          </cell>
-          <cell r="T55">
-            <v>23.34074029849074</v>
-          </cell>
         </row>
         <row r="56">
           <cell r="C56">
@@ -1693,15 +1639,6 @@
           <cell r="O56">
             <v>-1.2705465821244886</v>
           </cell>
-          <cell r="R56">
-            <v>6.8882153837909063E-2</v>
-          </cell>
-          <cell r="S56">
-            <v>0.47718038153733355</v>
-          </cell>
-          <cell r="T56">
-            <v>25.116103406269225</v>
-          </cell>
         </row>
         <row r="57">
           <cell r="C57">
@@ -1731,15 +1668,6 @@
           <cell r="O57">
             <v>15.149181622189108</v>
           </cell>
-          <cell r="R57">
-            <v>0.9381216481786423</v>
-          </cell>
-          <cell r="S57">
-            <v>0.5077645224650349</v>
-          </cell>
-          <cell r="T57">
-            <v>49.4462911948225</v>
-          </cell>
         </row>
         <row r="58">
           <cell r="C58">
@@ -1769,15 +1697,6 @@
           <cell r="O58">
             <v>18.416382111833716</v>
           </cell>
-          <cell r="R58">
-            <v>0.21979280255911871</v>
-          </cell>
-          <cell r="S58">
-            <v>0.51940745120897858</v>
-          </cell>
-          <cell r="T58">
-            <v>53.336180272097756</v>
-          </cell>
         </row>
         <row r="59">
           <cell r="C59">
@@ -1807,15 +1726,6 @@
           <cell r="O59">
             <v>-1126.0149500201239</v>
           </cell>
-          <cell r="R59">
-            <v>0.21193928714724924</v>
-          </cell>
-          <cell r="S59">
-            <v>0.40207406037581572</v>
-          </cell>
-          <cell r="T59">
-            <v>56.87230128020262</v>
-          </cell>
         </row>
         <row r="60">
           <cell r="C60">
@@ -1845,15 +1755,6 @@
           <cell r="O60">
             <v>17.772712882865964</v>
           </cell>
-          <cell r="R60">
-            <v>0.80054962134214658</v>
-          </cell>
-          <cell r="S60">
-            <v>0.57088290431277111</v>
-          </cell>
-          <cell r="T60">
-            <v>56.371812403237143</v>
-          </cell>
         </row>
         <row r="61">
           <cell r="C61">
@@ -1883,15 +1784,6 @@
           <cell r="O61">
             <v>-766.13796004513358</v>
           </cell>
-          <cell r="R61">
-            <v>0.24783374084777576</v>
-          </cell>
-          <cell r="S61">
-            <v>0.46349228615896698</v>
-          </cell>
-          <cell r="T61">
-            <v>23.733704875177946</v>
-          </cell>
         </row>
         <row r="62">
           <cell r="C62">
@@ -1921,15 +1813,6 @@
           <cell r="O62">
             <v>-11.762998582108743</v>
           </cell>
-          <cell r="R62">
-            <v>0.85084924788125105</v>
-          </cell>
-          <cell r="S62">
-            <v>0.57824543445205723</v>
-          </cell>
-          <cell r="T62">
-            <v>23.305024209757118</v>
-          </cell>
         </row>
         <row r="63">
           <cell r="C63">
@@ -1959,15 +1842,6 @@
           <cell r="O63">
             <v>-21.590970793867715</v>
           </cell>
-          <cell r="R63">
-            <v>0.82397390312715935</v>
-          </cell>
-          <cell r="S63">
-            <v>0.450631305942436</v>
-          </cell>
-          <cell r="T63">
-            <v>29.644057765331826</v>
-          </cell>
         </row>
         <row r="64">
           <cell r="C64">
@@ -1997,15 +1871,6 @@
           <cell r="O64">
             <v>21.81641022338372</v>
           </cell>
-          <cell r="R64">
-            <v>0.79902098567066893</v>
-          </cell>
-          <cell r="S64">
-            <v>0.59293662748582632</v>
-          </cell>
-          <cell r="T64">
-            <v>67.222486300510312</v>
-          </cell>
         </row>
         <row r="82">
           <cell r="C82">
@@ -2035,15 +1900,6 @@
           <cell r="O82">
             <v>55.487933815400687</v>
           </cell>
-          <cell r="R82">
-            <v>0.88227636311723401</v>
-          </cell>
-          <cell r="S82">
-            <v>0.50707291345847516</v>
-          </cell>
-          <cell r="T82">
-            <v>154.0591767836649</v>
-          </cell>
         </row>
         <row r="83">
           <cell r="C83">
@@ -2073,15 +1929,6 @@
           <cell r="O83">
             <v>63.293167537262505</v>
           </cell>
-          <cell r="R83">
-            <v>0.18790300159873752</v>
-          </cell>
-          <cell r="S83">
-            <v>0.57239085083930608</v>
-          </cell>
-          <cell r="T83">
-            <v>154.06046157396361</v>
-          </cell>
         </row>
         <row r="84">
           <cell r="C84">
@@ -2111,15 +1958,6 @@
           <cell r="O84">
             <v>-322.40567426948752</v>
           </cell>
-          <cell r="R84">
-            <v>0.76686864515872011</v>
-          </cell>
-          <cell r="S84">
-            <v>0.47204959495374793</v>
-          </cell>
-          <cell r="T84">
-            <v>134.18903533546296</v>
-          </cell>
         </row>
         <row r="85">
           <cell r="C85">
@@ -2149,15 +1987,6 @@
           <cell r="O85">
             <v>73.896908451333033</v>
           </cell>
-          <cell r="R85">
-            <v>0.13718531289149732</v>
-          </cell>
-          <cell r="S85">
-            <v>0.59630751102807489</v>
-          </cell>
-          <cell r="T85">
-            <v>199.65573034299604</v>
-          </cell>
         </row>
         <row r="86">
           <cell r="C86">
@@ -2187,15 +2016,6 @@
           <cell r="O86">
             <v>30.742882086794264</v>
           </cell>
-          <cell r="R86">
-            <v>0.20392839620411979</v>
-          </cell>
-          <cell r="S86">
-            <v>0.4667012427258016</v>
-          </cell>
-          <cell r="T86">
-            <v>119.85903158679552</v>
-          </cell>
         </row>
         <row r="87">
           <cell r="C87">
@@ -2225,15 +2045,6 @@
           <cell r="O87">
             <v>70.977269703510885</v>
           </cell>
-          <cell r="R87">
-            <v>0.18171346093995622</v>
-          </cell>
-          <cell r="S87">
-            <v>0.56472100018205351</v>
-          </cell>
-          <cell r="T87">
-            <v>174.64839262300603</v>
-          </cell>
         </row>
         <row r="88">
           <cell r="C88">
@@ -2263,15 +2074,6 @@
           <cell r="O88">
             <v>-363.65711748073318</v>
           </cell>
-          <cell r="R88">
-            <v>0.92250781324024145</v>
-          </cell>
-          <cell r="S88">
-            <v>0.56096194316368164</v>
-          </cell>
-          <cell r="T88">
-            <v>147.60037166857651</v>
-          </cell>
         </row>
         <row r="89">
           <cell r="C89">
@@ -2301,15 +2103,6 @@
           <cell r="O89">
             <v>63.367271595646905</v>
           </cell>
-          <cell r="R89">
-            <v>0.88076235560331151</v>
-          </cell>
-          <cell r="S89">
-            <v>0.58757462959722995</v>
-          </cell>
-          <cell r="T89">
-            <v>184.98558764893693</v>
-          </cell>
         </row>
         <row r="90">
           <cell r="C90">
@@ -2339,15 +2132,6 @@
           <cell r="O90">
             <v>63.734846789469508</v>
           </cell>
-          <cell r="R90">
-            <v>0.77065176419045534</v>
-          </cell>
-          <cell r="S90">
-            <v>0.56063354662824882</v>
-          </cell>
-          <cell r="T90">
-            <v>157.59165095675357</v>
-          </cell>
         </row>
         <row r="91">
           <cell r="C91">
@@ -2377,15 +2161,6 @@
           <cell r="O91">
             <v>-698.26859762179106</v>
           </cell>
-          <cell r="R91">
-            <v>6.271336723665151E-2</v>
-          </cell>
-          <cell r="S91">
-            <v>0.59117163289627128</v>
-          </cell>
-          <cell r="T91">
-            <v>151.37962335593355</v>
-          </cell>
         </row>
         <row r="92">
           <cell r="C92">
@@ -2415,15 +2190,6 @@
           <cell r="O92">
             <v>-178.7984750980267</v>
           </cell>
-          <cell r="R92">
-            <v>0.12743169517801592</v>
-          </cell>
-          <cell r="S92">
-            <v>0.43610392935579556</v>
-          </cell>
-          <cell r="T92">
-            <v>110.7528407138401</v>
-          </cell>
         </row>
         <row r="93">
           <cell r="C93">
@@ -2453,15 +2219,6 @@
           <cell r="O93">
             <v>-193.06839148325176</v>
           </cell>
-          <cell r="R93">
-            <v>0.87266310370394118</v>
-          </cell>
-          <cell r="S93">
-            <v>0.47490824131895348</v>
-          </cell>
-          <cell r="T93">
-            <v>136.79835053878909</v>
-          </cell>
         </row>
         <row r="94">
           <cell r="C94">
@@ -2491,15 +2248,6 @@
           <cell r="O94">
             <v>-263.33154635958152</v>
           </cell>
-          <cell r="R94">
-            <v>0.81827233923183262</v>
-          </cell>
-          <cell r="S94">
-            <v>0.52277278616433454</v>
-          </cell>
-          <cell r="T94">
-            <v>150.57280126077598</v>
-          </cell>
         </row>
         <row r="95">
           <cell r="C95">
@@ -2529,15 +2277,6 @@
           <cell r="O95">
             <v>65.957956470574771</v>
           </cell>
-          <cell r="R95">
-            <v>0.82731138128965387</v>
-          </cell>
-          <cell r="S95">
-            <v>0.47670985271811817</v>
-          </cell>
-          <cell r="T95">
-            <v>139.05616094543484</v>
-          </cell>
         </row>
         <row r="96">
           <cell r="C96">
@@ -2566,15 +2305,6 @@
           </cell>
           <cell r="O96">
             <v>51.810464269448588</v>
-          </cell>
-          <cell r="R96">
-            <v>8.2730807515312324E-2</v>
-          </cell>
-          <cell r="S96">
-            <v>0.50123084139536123</v>
-          </cell>
-          <cell r="T96">
-            <v>140.14954975333927</v>
           </cell>
         </row>
         <row r="98">
@@ -4310,7 +4040,7 @@
         <v>17</v>
       </c>
       <c r="V4">
-        <f t="shared" ref="V4:V47" si="6">1-T4</f>
+        <f t="shared" ref="V4:V32" si="6">1-T4</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="W4">
@@ -4409,7 +4139,7 @@
         <v>0.5</v>
       </c>
       <c r="W5">
-        <f t="shared" ref="W5:W47" si="7">S5*T5+U5*V5</f>
+        <f t="shared" ref="W5:W32" si="7">S5*T5+U5*V5</f>
         <v>11</v>
       </c>
       <c r="X5" s="3">
@@ -5014,8 +4744,7 @@
         <v>0.54</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
-        <v>25.180000000000003</v>
+        <v>25</v>
       </c>
       <c r="I12">
         <f>ROUND('[1]values '!H11,0)</f>
@@ -5079,7 +4808,7 @@
       </c>
       <c r="X12" s="3">
         <f t="shared" si="8"/>
-        <v>29.832499999999996</v>
+        <v>29.787500000000001</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
@@ -7053,28 +6782,23 @@
         <v>3.9499999999999815</v>
       </c>
       <c r="S33">
-        <f>ROUND('[1]values '!R50,0)</f>
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="T33">
-        <f>ROUND('[1]values '!S50,2)</f>
-        <v>0.45</v>
+        <v>0.15</v>
       </c>
       <c r="U33">
-        <f>ROUND('[1]values '!T50,0)</f>
         <v>13</v>
       </c>
       <c r="V33">
-        <f t="shared" si="6"/>
-        <v>0.55000000000000004</v>
+        <v>0.85</v>
       </c>
       <c r="W33">
-        <f t="shared" si="7"/>
-        <v>7.15</v>
+        <v>27.699999999999996</v>
       </c>
       <c r="X33" s="3">
         <f t="shared" si="8"/>
-        <v>4.3149999999999942</v>
+        <v>9.4524999999999935</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.35">
@@ -7148,28 +6872,23 @@
         <v>25.65</v>
       </c>
       <c r="S34">
-        <f>ROUND('[1]values '!R51,0)</f>
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="T34">
-        <f>ROUND('[1]values '!S51,2)</f>
-        <v>0.5</v>
+        <v>0.11</v>
       </c>
       <c r="U34">
-        <f>ROUND('[1]values '!T51,0)</f>
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="V34">
-        <f t="shared" si="6"/>
-        <v>0.5</v>
+        <v>0.89</v>
       </c>
       <c r="W34">
-        <f t="shared" si="7"/>
-        <v>27.5</v>
+        <v>17.939999999999998</v>
       </c>
       <c r="X34" s="3">
         <f t="shared" si="8"/>
-        <v>22.97</v>
+        <v>20.58</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.35">
@@ -7243,28 +6962,23 @@
         <v>9.7199999999999989</v>
       </c>
       <c r="S35">
-        <f>ROUND('[1]values '!R52,0)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="T35">
-        <f>ROUND('[1]values '!S52,2)</f>
-        <v>0.43</v>
+        <v>0.87</v>
       </c>
       <c r="U35">
-        <f>ROUND('[1]values '!T52,0)</f>
-        <v>20</v>
+        <v>-34</v>
       </c>
       <c r="V35">
-        <f t="shared" si="6"/>
-        <v>0.57000000000000006</v>
+        <v>0.13</v>
       </c>
       <c r="W35">
-        <f t="shared" si="7"/>
-        <v>11.400000000000002</v>
+        <v>14.72</v>
       </c>
       <c r="X35" s="3">
         <f t="shared" si="8"/>
-        <v>9.5399999999999991</v>
+        <v>10.37</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.35">
@@ -7338,28 +7052,23 @@
         <v>21.52</v>
       </c>
       <c r="S36">
-        <f>ROUND('[1]values '!R53,0)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="T36">
-        <f>ROUND('[1]values '!S53,2)</f>
-        <v>0.5</v>
+        <v>0.11</v>
       </c>
       <c r="U36">
-        <f>ROUND('[1]values '!T53,0)</f>
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="V36">
-        <f t="shared" si="6"/>
-        <v>0.5</v>
+        <v>0.89</v>
       </c>
       <c r="W36">
-        <f t="shared" si="7"/>
-        <v>23.5</v>
+        <v>10.86</v>
       </c>
       <c r="X36" s="3">
         <f t="shared" si="8"/>
-        <v>20.599999999999998</v>
+        <v>17.439999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.35">
@@ -7433,28 +7142,23 @@
         <v>9.7399999999999967</v>
       </c>
       <c r="S37">
-        <f>ROUND('[1]values '!R54,0)</f>
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="T37">
-        <f>ROUND('[1]values '!S54,2)</f>
-        <v>0.41</v>
+        <v>0.16</v>
       </c>
       <c r="U37">
-        <f>ROUND('[1]values '!T54,0)</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="V37">
-        <f t="shared" si="6"/>
-        <v>0.59000000000000008</v>
+        <v>0.84</v>
       </c>
       <c r="W37">
-        <f t="shared" si="7"/>
-        <v>10.440000000000001</v>
+        <v>31.799999999999997</v>
       </c>
       <c r="X37" s="3">
         <f t="shared" si="8"/>
-        <v>8.1849999999999987</v>
+        <v>13.524999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.35">
@@ -7528,28 +7232,23 @@
         <v>10.5</v>
       </c>
       <c r="S38">
-        <f>ROUND('[1]values '!R55,0)</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="T38">
-        <f>ROUND('[1]values '!S55,2)</f>
-        <v>0.45</v>
+        <v>0.82</v>
       </c>
       <c r="U38">
-        <f>ROUND('[1]values '!T55,0)</f>
-        <v>23</v>
+        <v>-212</v>
       </c>
       <c r="V38">
-        <f t="shared" si="6"/>
-        <v>0.55000000000000004</v>
+        <v>0.18000000000000005</v>
       </c>
       <c r="W38">
-        <f t="shared" si="7"/>
-        <v>12.65</v>
+        <v>31.539999999999992</v>
       </c>
       <c r="X38" s="3">
         <f t="shared" si="8"/>
-        <v>10.565</v>
+        <v>15.287499999999998</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.35">
@@ -7623,28 +7322,23 @@
         <v>10.399999999999999</v>
       </c>
       <c r="S39">
-        <f>ROUND('[1]values '!R56,0)</f>
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="T39">
-        <f>ROUND('[1]values '!S56,2)</f>
-        <v>0.48</v>
+        <v>0.94</v>
       </c>
       <c r="U39">
-        <f>ROUND('[1]values '!T56,0)</f>
-        <v>25</v>
+        <v>-896</v>
       </c>
       <c r="V39">
-        <f t="shared" si="6"/>
-        <v>0.52</v>
+        <v>6.0000000000000053E-2</v>
       </c>
       <c r="W39">
-        <f t="shared" si="7"/>
-        <v>13</v>
+        <v>32.719999999999942</v>
       </c>
       <c r="X39" s="3">
         <f t="shared" si="8"/>
-        <v>9.1875</v>
+        <v>14.117499999999986</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.35">
@@ -7718,28 +7412,23 @@
         <v>21.93</v>
       </c>
       <c r="S40">
-        <f>ROUND('[1]values '!R57,0)</f>
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="T40">
-        <f>ROUND('[1]values '!S57,2)</f>
-        <v>0.51</v>
+        <v>0.76</v>
       </c>
       <c r="U40">
-        <f>ROUND('[1]values '!T57,0)</f>
-        <v>49</v>
+        <v>-185</v>
       </c>
       <c r="V40">
-        <f t="shared" si="6"/>
-        <v>0.49</v>
+        <v>0.24</v>
       </c>
       <c r="W40">
-        <f t="shared" si="7"/>
-        <v>24.52</v>
+        <v>23.240000000000002</v>
       </c>
       <c r="X40" s="3">
         <f t="shared" si="8"/>
-        <v>20.115000000000006</v>
+        <v>19.795000000000005</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.35">
@@ -7813,28 +7502,23 @@
         <v>21.119999999999997</v>
       </c>
       <c r="S41">
-        <f>ROUND('[1]values '!R58,0)</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="T41">
-        <f>ROUND('[1]values '!S58,2)</f>
-        <v>0.52</v>
+        <v>0.08</v>
       </c>
       <c r="U41">
-        <f>ROUND('[1]values '!T58,0)</f>
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="V41">
-        <f t="shared" si="6"/>
-        <v>0.48</v>
+        <v>0.92</v>
       </c>
       <c r="W41">
-        <f t="shared" si="7"/>
-        <v>25.439999999999998</v>
+        <v>21.96</v>
       </c>
       <c r="X41" s="3">
         <f t="shared" si="8"/>
-        <v>20.737500000000001</v>
+        <v>19.8675</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.35">
@@ -7908,28 +7592,23 @@
         <v>33.710000000000051</v>
       </c>
       <c r="S42">
-        <f>ROUND('[1]values '!R59,0)</f>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="T42">
-        <f>ROUND('[1]values '!S59,2)</f>
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="U42">
-        <f>ROUND('[1]values '!T59,0)</f>
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="V42">
-        <f t="shared" si="6"/>
-        <v>0.6</v>
+        <v>0.78</v>
       </c>
       <c r="W42">
-        <f t="shared" si="7"/>
-        <v>34.199999999999996</v>
+        <v>16.68</v>
       </c>
       <c r="X42" s="3">
         <f t="shared" si="8"/>
-        <v>30.122500000000009</v>
+        <v>25.742500000000014</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.35">
@@ -8003,28 +7682,23 @@
         <v>20.89</v>
       </c>
       <c r="S43">
-        <f>ROUND('[1]values '!R60,0)</f>
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="T43">
-        <f>ROUND('[1]values '!S60,2)</f>
-        <v>0.56999999999999995</v>
+        <v>0.86</v>
       </c>
       <c r="U43">
-        <f>ROUND('[1]values '!T60,0)</f>
-        <v>56</v>
+        <v>-265</v>
       </c>
       <c r="V43">
-        <f t="shared" si="6"/>
-        <v>0.43000000000000005</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="W43">
-        <f t="shared" si="7"/>
-        <v>24.650000000000002</v>
+        <v>11.919999999999995</v>
       </c>
       <c r="X43" s="3">
         <f t="shared" si="8"/>
-        <v>20.79</v>
+        <v>17.607499999999998</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.35">
@@ -8098,28 +7772,23 @@
         <v>14.160000000000025</v>
       </c>
       <c r="S44">
-        <f>ROUND('[1]values '!R61,0)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="T44">
-        <f>ROUND('[1]values '!S61,2)</f>
-        <v>0.46</v>
+        <v>0.79</v>
       </c>
       <c r="U44">
-        <f>ROUND('[1]values '!T61,0)</f>
-        <v>24</v>
+        <v>-118</v>
       </c>
       <c r="V44">
-        <f t="shared" si="6"/>
-        <v>0.54</v>
+        <v>0.20999999999999996</v>
       </c>
       <c r="W44">
-        <f t="shared" si="7"/>
-        <v>12.96</v>
+        <v>18.670000000000009</v>
       </c>
       <c r="X44" s="3">
         <f t="shared" si="8"/>
-        <v>11.024999999999995</v>
+        <v>12.452499999999997</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.35">
@@ -8193,28 +7862,23 @@
         <v>8.3999999999999986</v>
       </c>
       <c r="S45">
-        <f>ROUND('[1]values '!R62,0)</f>
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="T45">
-        <f>ROUND('[1]values '!S62,2)</f>
-        <v>0.57999999999999996</v>
+        <v>0.15</v>
       </c>
       <c r="U45">
-        <f>ROUND('[1]values '!T62,0)</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V45">
-        <f t="shared" si="6"/>
-        <v>0.42000000000000004</v>
+        <v>0.85</v>
       </c>
       <c r="W45">
-        <f t="shared" si="7"/>
-        <v>10.24</v>
+        <v>22.75</v>
       </c>
       <c r="X45" s="3">
         <f t="shared" si="8"/>
-        <v>6.7449999999999974</v>
+        <v>9.8724999999999987</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.35">
@@ -8288,28 +7952,23 @@
         <v>14.079999999999998</v>
       </c>
       <c r="S46">
-        <f>ROUND('[1]values '!R63,0)</f>
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="T46">
-        <f>ROUND('[1]values '!S63,2)</f>
-        <v>0.45</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="U46">
-        <f>ROUND('[1]values '!T63,0)</f>
-        <v>30</v>
+        <v>-2</v>
       </c>
       <c r="V46">
-        <f t="shared" si="6"/>
-        <v>0.55000000000000004</v>
+        <v>0.86</v>
       </c>
       <c r="W46">
-        <f t="shared" si="7"/>
-        <v>16.95</v>
+        <v>7.5200000000000005</v>
       </c>
       <c r="X46" s="3">
         <f t="shared" si="8"/>
-        <v>13.515000000000008</v>
+        <v>11.157500000000008</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.35">
@@ -8383,28 +8042,23 @@
         <v>27.34</v>
       </c>
       <c r="S47">
-        <f>ROUND('[1]values '!R64,0)</f>
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="T47">
-        <f>ROUND('[1]values '!S64,2)</f>
-        <v>0.59</v>
+        <v>0.82</v>
       </c>
       <c r="U47">
-        <f>ROUND('[1]values '!T64,0)</f>
-        <v>67</v>
+        <v>-140</v>
       </c>
       <c r="V47">
-        <f t="shared" si="6"/>
-        <v>0.41000000000000003</v>
+        <v>0.18000000000000005</v>
       </c>
       <c r="W47">
-        <f t="shared" si="7"/>
-        <v>28.060000000000002</v>
+        <v>21.539999999999988</v>
       </c>
       <c r="X47" s="3">
         <f t="shared" si="8"/>
-        <v>26.557500000000001</v>
+        <v>24.927499999999998</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.35">
@@ -8478,28 +8132,23 @@
         <v>71.52</v>
       </c>
       <c r="S48">
-        <f>ROUND('[1]values '!R82,0)</f>
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="T48">
-        <f>ROUND('[1]values '!S82,2)</f>
-        <v>0.51</v>
+        <v>0.89</v>
       </c>
       <c r="U48">
-        <f>ROUND('[1]values '!T82,0)</f>
-        <v>154</v>
+        <v>-136</v>
       </c>
       <c r="V48">
-        <f t="shared" ref="V48:V78" si="15">1-T48</f>
-        <v>0.49</v>
+        <v>0.10999999999999999</v>
       </c>
       <c r="W48">
-        <f t="shared" ref="W48:W78" si="16">S48*T48+U48*V48</f>
-        <v>75.97</v>
+        <v>73.150000000000006</v>
       </c>
       <c r="X48" s="3">
         <f t="shared" si="8"/>
-        <v>70.66749999999999</v>
+        <v>69.962499999999977</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.35">
@@ -8573,28 +8222,23 @@
         <v>64.7</v>
       </c>
       <c r="S49">
-        <f>ROUND('[1]values '!R83,0)</f>
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="T49">
-        <f>ROUND('[1]values '!S83,2)</f>
-        <v>0.56999999999999995</v>
+        <v>0.95</v>
       </c>
       <c r="U49">
-        <f>ROUND('[1]values '!T83,0)</f>
-        <v>154</v>
+        <v>-39</v>
       </c>
       <c r="V49">
-        <f t="shared" si="15"/>
-        <v>0.43000000000000005</v>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="W49">
-        <f t="shared" si="16"/>
-        <v>66.220000000000013</v>
+        <v>71.199999999999989</v>
       </c>
       <c r="X49" s="3">
         <f t="shared" si="8"/>
-        <v>64.690000000000012</v>
+        <v>65.935000000000002</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.35">
@@ -8668,28 +8312,23 @@
         <v>68.099999999999966</v>
       </c>
       <c r="S50">
-        <f>ROUND('[1]values '!R84,0)</f>
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="T50">
-        <f>ROUND('[1]values '!S84,2)</f>
-        <v>0.47</v>
+        <v>0.95</v>
       </c>
       <c r="U50">
-        <f>ROUND('[1]values '!T84,0)</f>
-        <v>134</v>
+        <v>-589</v>
       </c>
       <c r="V50">
-        <f t="shared" si="15"/>
-        <v>0.53</v>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="W50">
-        <f t="shared" si="16"/>
-        <v>71.490000000000009</v>
+        <v>81.69999999999996</v>
       </c>
       <c r="X50" s="3">
         <f t="shared" si="8"/>
-        <v>65.974999999999994</v>
+        <v>68.527499999999975</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.35">
@@ -8763,28 +8402,23 @@
         <v>76.8</v>
       </c>
       <c r="S51">
-        <f>ROUND('[1]values '!R85,0)</f>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="T51">
-        <f>ROUND('[1]values '!S85,2)</f>
-        <v>0.6</v>
+        <v>0.87</v>
       </c>
       <c r="U51">
-        <f>ROUND('[1]values '!T85,0)</f>
-        <v>200</v>
+        <v>-28</v>
       </c>
       <c r="V51">
-        <f t="shared" si="15"/>
-        <v>0.4</v>
+        <v>0.13</v>
       </c>
       <c r="W51">
-        <f t="shared" si="16"/>
-        <v>80</v>
+        <v>55.519999999999996</v>
       </c>
       <c r="X51" s="3">
         <f t="shared" si="8"/>
-        <v>75.642500000000013</v>
+        <v>69.522500000000008</v>
       </c>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.35">
@@ -8858,28 +8492,23 @@
         <v>61.78</v>
       </c>
       <c r="S52">
-        <f>ROUND('[1]values '!R86,0)</f>
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="T52">
-        <f>ROUND('[1]values '!S86,2)</f>
-        <v>0.47</v>
+        <v>0.92</v>
       </c>
       <c r="U52">
-        <f>ROUND('[1]values '!T86,0)</f>
-        <v>120</v>
+        <v>-710</v>
       </c>
       <c r="V52">
-        <f t="shared" si="15"/>
-        <v>0.53</v>
+        <v>7.999999999999996E-2</v>
       </c>
       <c r="W52">
-        <f t="shared" si="16"/>
-        <v>63.6</v>
+        <v>80.280000000000044</v>
       </c>
       <c r="X52" s="3">
         <f t="shared" si="8"/>
-        <v>61.63</v>
+        <v>65.800000000000011</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.35">
@@ -8953,28 +8582,23 @@
         <v>75.27</v>
       </c>
       <c r="S53">
-        <f>ROUND('[1]values '!R87,0)</f>
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="T53">
-        <f>ROUND('[1]values '!S87,2)</f>
-        <v>0.56000000000000005</v>
+        <v>0.78</v>
       </c>
       <c r="U53">
-        <f>ROUND('[1]values '!T87,0)</f>
-        <v>175</v>
+        <v>-260</v>
       </c>
       <c r="V53">
-        <f t="shared" si="15"/>
-        <v>0.43999999999999995</v>
+        <v>0.21999999999999997</v>
       </c>
       <c r="W53">
-        <f t="shared" si="16"/>
-        <v>76.999999999999986</v>
+        <v>74.62</v>
       </c>
       <c r="X53" s="3">
         <f t="shared" si="8"/>
-        <v>73.057500000000005</v>
+        <v>72.462500000000006</v>
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.35">
@@ -9048,28 +8672,23 @@
         <v>63.169999999999995</v>
       </c>
       <c r="S54">
-        <f>ROUND('[1]values '!R88,0)</f>
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="T54">
-        <f>ROUND('[1]values '!S88,2)</f>
-        <v>0.56000000000000005</v>
+        <v>0.86</v>
       </c>
       <c r="U54">
-        <f>ROUND('[1]values '!T88,0)</f>
-        <v>148</v>
+        <v>-102</v>
       </c>
       <c r="V54">
-        <f t="shared" si="15"/>
-        <v>0.43999999999999995</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="W54">
-        <f t="shared" si="16"/>
-        <v>65.679999999999993</v>
+        <v>70</v>
       </c>
       <c r="X54" s="3">
         <f t="shared" si="8"/>
-        <v>63.034999999999997</v>
+        <v>64.114999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.35">
@@ -9143,28 +8762,23 @@
         <v>72.23</v>
       </c>
       <c r="S55">
-        <f>ROUND('[1]values '!R89,0)</f>
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="T55">
-        <f>ROUND('[1]values '!S89,2)</f>
-        <v>0.59</v>
+        <v>0.09</v>
       </c>
       <c r="U55">
-        <f>ROUND('[1]values '!T89,0)</f>
-        <v>185</v>
+        <v>76</v>
       </c>
       <c r="V55">
-        <f t="shared" si="15"/>
-        <v>0.41000000000000003</v>
+        <v>0.91</v>
       </c>
       <c r="W55">
-        <f t="shared" si="16"/>
-        <v>76.440000000000012</v>
+        <v>77.89</v>
       </c>
       <c r="X55" s="3">
         <f t="shared" si="8"/>
-        <v>71.790000000000006</v>
+        <v>72.152500000000003</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.35">
@@ -9238,28 +8852,23 @@
         <v>65.92</v>
       </c>
       <c r="S56">
-        <f>ROUND('[1]values '!R90,0)</f>
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="T56">
-        <f>ROUND('[1]values '!S90,2)</f>
-        <v>0.56000000000000005</v>
+        <v>0.89</v>
       </c>
       <c r="U56">
-        <f>ROUND('[1]values '!T90,0)</f>
-        <v>158</v>
+        <v>-457</v>
       </c>
       <c r="V56">
-        <f t="shared" si="15"/>
-        <v>0.43999999999999995</v>
+        <v>0.10999999999999999</v>
       </c>
       <c r="W56">
-        <f t="shared" si="16"/>
-        <v>70.08</v>
+        <v>60.980000000000004</v>
       </c>
       <c r="X56" s="3">
         <f t="shared" si="8"/>
-        <v>65.457499999999996</v>
+        <v>63.182500000000005</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.35">
@@ -9333,28 +8942,23 @@
         <v>58.000000000000014</v>
       </c>
       <c r="S57">
-        <f>ROUND('[1]values '!R91,0)</f>
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="T57">
-        <f>ROUND('[1]values '!S91,2)</f>
-        <v>0.59</v>
+        <v>0.23</v>
       </c>
       <c r="U57">
-        <f>ROUND('[1]values '!T91,0)</f>
-        <v>151</v>
+        <v>53</v>
       </c>
       <c r="V57">
-        <f t="shared" si="15"/>
-        <v>0.41000000000000003</v>
+        <v>0.77</v>
       </c>
       <c r="W57">
-        <f t="shared" si="16"/>
-        <v>61.910000000000004</v>
+        <v>68.180000000000007</v>
       </c>
       <c r="X57" s="3">
         <f t="shared" si="8"/>
-        <v>56.672500000000007</v>
+        <v>58.240000000000009</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.35">
@@ -9428,28 +9032,23 @@
         <v>60.08</v>
       </c>
       <c r="S58">
-        <f>ROUND('[1]values '!R92,0)</f>
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="T58">
-        <f>ROUND('[1]values '!S92,2)</f>
-        <v>0.44</v>
+        <v>0.17</v>
       </c>
       <c r="U58">
-        <f>ROUND('[1]values '!T92,0)</f>
-        <v>111</v>
+        <v>73</v>
       </c>
       <c r="V58">
-        <f t="shared" si="15"/>
-        <v>0.56000000000000005</v>
+        <v>0.83</v>
       </c>
       <c r="W58">
-        <f t="shared" si="16"/>
-        <v>62.160000000000004</v>
+        <v>73.679999999999993</v>
       </c>
       <c r="X58" s="3">
         <f t="shared" si="8"/>
-        <v>58.407500000000006</v>
+        <v>61.287500000000009</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.35">
@@ -9523,28 +9122,23 @@
         <v>70.200000000000017</v>
       </c>
       <c r="S59">
-        <f>ROUND('[1]values '!R93,0)</f>
-        <v>1</v>
+        <v>151</v>
       </c>
       <c r="T59">
-        <f>ROUND('[1]values '!S93,2)</f>
-        <v>0.47</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="U59">
-        <f>ROUND('[1]values '!T93,0)</f>
-        <v>137</v>
+        <v>48</v>
       </c>
       <c r="V59">
-        <f t="shared" si="15"/>
-        <v>0.53</v>
+        <v>0.86</v>
       </c>
       <c r="W59">
-        <f t="shared" si="16"/>
-        <v>73.08</v>
+        <v>62.42</v>
       </c>
       <c r="X59" s="3">
         <f t="shared" si="8"/>
-        <v>68.38000000000001</v>
+        <v>65.715000000000003</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.35">
@@ -9618,28 +9212,23 @@
         <v>69.100000000000009</v>
       </c>
       <c r="S60">
-        <f>ROUND('[1]values '!R94,0)</f>
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="T60">
-        <f>ROUND('[1]values '!S94,2)</f>
-        <v>0.52</v>
+        <v>0.78</v>
       </c>
       <c r="U60">
-        <f>ROUND('[1]values '!T94,0)</f>
-        <v>151</v>
+        <v>-244</v>
       </c>
       <c r="V60">
-        <f t="shared" si="15"/>
-        <v>0.48</v>
+        <v>0.21999999999999997</v>
       </c>
       <c r="W60">
-        <f t="shared" si="16"/>
-        <v>73</v>
+        <v>72.680000000000007</v>
       </c>
       <c r="X60" s="3">
         <f t="shared" si="8"/>
-        <v>68.37</v>
+        <v>68.290000000000006</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.35">
@@ -9713,28 +9302,23 @@
         <v>71.34</v>
       </c>
       <c r="S61">
-        <f>ROUND('[1]values '!R95,0)</f>
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="T61">
-        <f>ROUND('[1]values '!S95,2)</f>
-        <v>0.48</v>
+        <v>0.19</v>
       </c>
       <c r="U61">
-        <f>ROUND('[1]values '!T95,0)</f>
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="V61">
-        <f t="shared" si="15"/>
-        <v>0.52</v>
+        <v>0.81</v>
       </c>
       <c r="W61">
-        <f t="shared" si="16"/>
-        <v>72.760000000000005</v>
+        <v>81.44</v>
       </c>
       <c r="X61" s="3">
         <f t="shared" si="8"/>
-        <v>70.310000000000016</v>
+        <v>72.480000000000018</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.35">
@@ -9808,28 +9392,23 @@
         <v>66.84</v>
       </c>
       <c r="S62">
-        <f>ROUND('[1]values '!R96,0)</f>
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="T62">
-        <f>ROUND('[1]values '!S96,2)</f>
-        <v>0.5</v>
+        <v>0.83</v>
       </c>
       <c r="U62">
-        <f>ROUND('[1]values '!T96,0)</f>
-        <v>140</v>
+        <v>-190</v>
       </c>
       <c r="V62">
-        <f t="shared" si="15"/>
-        <v>0.5</v>
+        <v>0.17000000000000004</v>
       </c>
       <c r="W62">
-        <f t="shared" si="16"/>
-        <v>70</v>
+        <v>61.489999999999988</v>
       </c>
       <c r="X62" s="3">
         <f t="shared" si="8"/>
-        <v>65.11</v>
+        <v>62.982499999999995</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.35">
@@ -9915,11 +9494,11 @@
         <v>1</v>
       </c>
       <c r="V63">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="V63:V78" si="15">1-T63</f>
         <v>0.59000000000000008</v>
       </c>
       <c r="W63">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="W63:W78" si="16">S63*T63+U63*V63</f>
         <v>7.1499999999999995</v>
       </c>
       <c r="X63" s="3">

</xml_diff>